<commit_message>
Two sets of upload tests needed to be in different projects in order for them to pass. All tests passing.
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7C477B-B4EA-314A-B1EB-3606F42C60BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BBF85E-08AF-FF4D-9CEF-0C66B36E1386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="7060" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="5800" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Server</t>
   </si>
   <si>
-    <t>https://localhost:8080</t>
-  </si>
-  <si>
     <t>Scans</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Directory</t>
+  </si>
+  <si>
+    <t>http://localhost:8080</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,22 +482,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typo in fixtures spreadsheet
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BBF85E-08AF-FF4D-9CEF-0C66B36E1386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB164F0-DC15-374F-B2E7-3E991FC4EE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5800" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="2500" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -87,10 +87,10 @@
     <t>DICOM:StudyDate</t>
   </si>
   <si>
+    <t>http://localhost:8080</t>
+  </si>
+  <si>
     <t>Directory</t>
-  </si>
-  <si>
-    <t>http://localhost:8080</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DICOM parameters now have DICOM: prefix again, and XNATFileMatch moved to the dicoms.py to be close to the extraction function
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFA61FB-C0FA-C04A-AC3E-C71590AEDCF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF296B95-15B7-0E48-96BA-1411539B51E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42000" yWindow="1760" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,13 +84,13 @@
     <t>{Directory}</t>
   </si>
   <si>
+    <t>DICOM:StudyDate</t>
+  </si>
+  <si>
     <t>http://localhost:8080</t>
   </si>
   <si>
     <t>Directory</t>
-  </si>
-  <si>
-    <t>StudyDate</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added config section XNAT / AllowFields for configuring anonymisation
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF296B95-15B7-0E48-96BA-1411539B51E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FFF1EF-A19C-B04F-9519-D30C6FAC4408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42000" yWindow="1760" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14860" yWindow="2020" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Recipe</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Directory</t>
+  </si>
+  <si>
+    <t>AllowFields</t>
+  </si>
+  <si>
+    <t>AccessionNumber</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE643B-0B72-8E46-99FC-7188AD10E0D6}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,6 +550,14 @@
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
anonymisation rules are being applied from config
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FFF1EF-A19C-B04F-9519-D30C6FAC4408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44544546-CA3F-8444-956C-253480D49E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14860" yWindow="2020" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
     <t>AllowFields</t>
   </si>
   <si>
-    <t>AccessionNumber</t>
+    <t>StudyDate,AccessionNumber</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a "metadata" section to config to allow session_label to be configured rather than hard-coded
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_init.xlsx
+++ b/tests/fixtures/basic_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44544546-CA3F-8444-956C-253480D49E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35452788-6CEC-4141-9D64-17DDB996F030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="2020" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="2020" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Recipe</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>StudyDate,AccessionNumber</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>session_label</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE643B-0B72-8E46-99FC-7188AD10E0D6}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -533,36 +539,53 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{F33D5B97-A1A2-BF47-98A4-E6AE6E16313F}"/>
+    <hyperlink ref="C14" r:id="rId1" xr:uid="{F33D5B97-A1A2-BF47-98A4-E6AE6E16313F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>